<commit_message>
icon scene / farm / tower upgrades
</commit_message>
<xml_diff>
--- a/CS408 Level Design.xlsx
+++ b/CS408 Level Design.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58">
   <si>
     <t>CS 408 Tower Defense Level / Monsters / Towers</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Level 3: Beach</t>
   </si>
   <si>
+    <t>Towers</t>
+  </si>
+  <si>
     <t>Wave 1</t>
   </si>
   <si>
@@ -46,12 +49,27 @@
     <t>Lv 1 Slime</t>
   </si>
   <si>
+    <t>Gun Tower</t>
+  </si>
+  <si>
+    <t>AOE Tower</t>
+  </si>
+  <si>
+    <t>Blade Tower</t>
+  </si>
+  <si>
+    <t>Farm</t>
+  </si>
+  <si>
     <t>Wave 2</t>
   </si>
   <si>
     <t>Lv 1 Bat</t>
   </si>
   <si>
+    <t>Cost</t>
+  </si>
+  <si>
     <t>Wave 3</t>
   </si>
   <si>
@@ -73,6 +91,9 @@
     <t>Lv 1 Flying Fire</t>
   </si>
   <si>
+    <t>Sell</t>
+  </si>
+  <si>
     <t>Wave 6</t>
   </si>
   <si>
@@ -91,6 +112,9 @@
     <t>Boss Barbarian</t>
   </si>
   <si>
+    <t>Damage</t>
+  </si>
+  <si>
     <t>Wave 9</t>
   </si>
   <si>
@@ -112,6 +136,9 @@
     <t>Wave 11</t>
   </si>
   <si>
+    <t>Range</t>
+  </si>
+  <si>
     <t>Wave 12</t>
   </si>
   <si>
@@ -133,6 +160,9 @@
     <t>Lv 2 Flying Fire</t>
   </si>
   <si>
+    <t>Fire Rate</t>
+  </si>
+  <si>
     <t>Wave 15</t>
   </si>
   <si>
@@ -143,6 +173,9 @@
   </si>
   <si>
     <t>Wave 17</t>
+  </si>
+  <si>
+    <t>DPS</t>
   </si>
   <si>
     <t>Wave 18</t>
@@ -163,9 +196,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -205,31 +238,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,21 +253,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,8 +281,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,6 +305,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,9 +359,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,22 +375,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -357,187 +390,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -606,17 +639,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -632,6 +659,36 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -670,36 +727,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -717,134 +750,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -879,9 +912,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1206,10 +1236,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1228,6 +1258,9 @@
     <col min="13" max="13" width="11.4285714285714" customWidth="1"/>
     <col min="14" max="14" width="14.8571428571429" customWidth="1"/>
     <col min="15" max="15" width="7.57142857142857" customWidth="1"/>
+    <col min="22" max="22" width="11.5714285714286" customWidth="1"/>
+    <col min="23" max="23" width="11.1428571428571" customWidth="1"/>
+    <col min="24" max="24" width="11.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1235,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="18.75" spans="1:17">
+    <row r="3" ht="18.75" spans="1:21">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1276,13 +1309,16 @@
       <c r="Q3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="U3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>30</v>
@@ -1294,10 +1330,10 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I4" s="3">
         <v>100</v>
@@ -1309,10 +1345,10 @@
         <v>3</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O4" s="3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="P4" s="3">
         <v>0.065</v>
@@ -1323,13 +1359,25 @@
       <c r="R4" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="V4" t="s">
+        <v>11</v>
+      </c>
+      <c r="W4" t="s">
+        <v>12</v>
+      </c>
+      <c r="X4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C5" s="3">
         <v>100</v>
@@ -1341,10 +1389,10 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I5" s="3">
         <v>40</v>
@@ -1356,13 +1404,13 @@
         <v>3</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O5" s="3">
         <v>100</v>
       </c>
       <c r="P5" s="3">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="Q5" s="3">
         <v>10</v>
@@ -1370,13 +1418,28 @@
       <c r="R5" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="U5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5">
+        <v>50</v>
+      </c>
+      <c r="W5">
+        <v>80</v>
+      </c>
+      <c r="X5">
+        <v>75</v>
+      </c>
+      <c r="Y5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5">
         <v>45</v>
@@ -1388,10 +1451,10 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I6" s="3">
         <v>30</v>
@@ -1403,13 +1466,13 @@
         <v>4</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O6" s="3">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="P6" s="3">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="Q6" s="3">
         <v>3</v>
@@ -1417,13 +1480,25 @@
       <c r="R6" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="V6">
+        <v>100</v>
+      </c>
+      <c r="W6">
+        <v>160</v>
+      </c>
+      <c r="X6">
+        <v>150</v>
+      </c>
+      <c r="Y6">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3">
         <v>30</v>
@@ -1435,10 +1510,10 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I7" s="3">
         <v>100</v>
@@ -1450,10 +1525,10 @@
         <v>50</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="O7" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="P7" s="3">
         <v>0.07</v>
@@ -1464,13 +1539,25 @@
       <c r="R7" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="V7">
+        <v>150</v>
+      </c>
+      <c r="W7">
+        <v>240</v>
+      </c>
+      <c r="X7">
+        <v>225</v>
+      </c>
+      <c r="Y7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5">
         <v>85</v>
@@ -1482,10 +1569,10 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I8" s="3">
         <v>50</v>
@@ -1497,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="O8" s="3">
         <v>100</v>
@@ -1511,13 +1598,28 @@
       <c r="R8" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="U8" t="s">
+        <v>25</v>
+      </c>
+      <c r="V8">
+        <v>25</v>
+      </c>
+      <c r="W8">
+        <v>40</v>
+      </c>
+      <c r="X8">
+        <v>40</v>
+      </c>
+      <c r="Y8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>100</v>
@@ -1529,10 +1631,10 @@
         <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I9" s="5">
         <v>85</v>
@@ -1544,7 +1646,7 @@
         <v>10</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="O9" s="5">
         <v>45</v>
@@ -1558,13 +1660,25 @@
       <c r="R9" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="V9">
+        <v>50</v>
+      </c>
+      <c r="W9">
+        <v>80</v>
+      </c>
+      <c r="X9">
+        <v>75</v>
+      </c>
+      <c r="Y9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" spans="1:25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3">
         <v>50</v>
@@ -1576,10 +1690,10 @@
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I10" s="3">
         <v>30</v>
@@ -1591,7 +1705,7 @@
         <v>2</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="O10" s="10">
         <v>85</v>
@@ -1602,16 +1716,28 @@
       <c r="Q10" s="10">
         <v>10</v>
       </c>
-      <c r="R10" s="13">
+      <c r="R10" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="V10">
+        <v>75</v>
+      </c>
+      <c r="W10">
+        <v>120</v>
+      </c>
+      <c r="X10">
+        <v>115</v>
+      </c>
+      <c r="Y10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C11" s="3">
         <v>75</v>
@@ -1623,10 +1749,10 @@
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="I11" s="7">
         <v>750</v>
@@ -1639,10 +1765,10 @@
         <v>1</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="O11" s="5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="P11" s="5">
         <v>0.065</v>
@@ -1653,13 +1779,25 @@
       <c r="R11" s="12">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="U11" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11">
+        <v>14</v>
+      </c>
+      <c r="W11">
+        <v>20</v>
+      </c>
+      <c r="Y11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3">
         <v>200</v>
@@ -1671,10 +1809,10 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I12" s="3">
         <v>75</v>
@@ -1686,13 +1824,13 @@
         <v>6</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="O12" s="3">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="P12" s="3">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="Q12" s="3">
         <v>10</v>
@@ -1700,13 +1838,22 @@
       <c r="R12" s="12">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="V12">
+        <v>22</v>
+      </c>
+      <c r="W12">
+        <v>30</v>
+      </c>
+      <c r="Y12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C13" s="7">
         <v>750</v>
@@ -1721,10 +1868,10 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="I13" s="3">
         <v>55</v>
@@ -1736,13 +1883,13 @@
         <v>5</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="O13" s="3">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="P13" s="3">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="Q13" s="3">
         <v>8</v>
@@ -1750,13 +1897,22 @@
       <c r="R13" s="12">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="7:18">
+      <c r="V13">
+        <v>30</v>
+      </c>
+      <c r="W13">
+        <v>40</v>
+      </c>
+      <c r="Y13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="7:23">
       <c r="G14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="I14" s="3">
         <v>200</v>
@@ -1768,7 +1924,7 @@
         <v>10</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="O14" s="3">
         <v>55</v>
@@ -1782,13 +1938,22 @@
       <c r="R14" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="7:18">
+      <c r="U14" t="s">
+        <v>40</v>
+      </c>
+      <c r="V14">
+        <v>10</v>
+      </c>
+      <c r="W14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="7:23">
       <c r="G15" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I15" s="5">
         <v>50</v>
@@ -1800,7 +1965,7 @@
         <v>4</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="O15" s="3">
         <v>180</v>
@@ -1814,10 +1979,16 @@
       <c r="R15" s="12">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" ht="18.75" spans="1:18">
+      <c r="V15">
+        <v>12</v>
+      </c>
+      <c r="W15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" ht="18.75" spans="1:23">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1832,10 +2003,10 @@
         <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="I16" s="3">
         <v>175</v>
@@ -1847,7 +2018,7 @@
         <v>65</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="O16" s="3">
         <v>75</v>
@@ -1858,16 +2029,22 @@
       <c r="Q16" s="3">
         <v>6</v>
       </c>
-      <c r="R16" s="13">
+      <c r="R16" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="V16">
+        <v>14</v>
+      </c>
+      <c r="W16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" spans="1:25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C17" s="3">
         <v>40</v>
@@ -1879,10 +2056,10 @@
         <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="I17" s="7">
         <v>1200</v>
@@ -1895,10 +2072,10 @@
         <v>1</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="O17" s="10">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="P17" s="10">
         <v>0.05</v>
@@ -1909,13 +2086,25 @@
       <c r="R17" s="12">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="U17" t="s">
+        <v>48</v>
+      </c>
+      <c r="V17">
+        <v>1.3</v>
+      </c>
+      <c r="W17">
+        <v>0.5</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
         <v>50</v>
@@ -1927,10 +2116,10 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="I18" s="3">
         <v>55</v>
@@ -1942,7 +2131,7 @@
         <v>5</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="O18" s="3">
         <v>750</v>
@@ -1953,13 +2142,22 @@
       <c r="R18" s="12">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="V18">
+        <v>1.5</v>
+      </c>
+      <c r="W18">
+        <v>0.5</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C19" s="3">
         <v>40</v>
@@ -1971,10 +2169,10 @@
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I19" s="3">
         <v>75</v>
@@ -1986,7 +2184,7 @@
         <v>6</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="O19" s="3">
         <v>850</v>
@@ -1997,13 +2195,22 @@
       <c r="R19" s="12">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="V19">
+        <v>1.7</v>
+      </c>
+      <c r="W19">
+        <v>0.5</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C20" s="5">
         <v>85</v>
@@ -2015,10 +2222,10 @@
         <v>10</v>
       </c>
       <c r="G20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I20" s="3">
         <v>180</v>
@@ -2030,7 +2237,7 @@
         <v>75</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="O20" s="3">
         <v>750</v>
@@ -2038,16 +2245,31 @@
       <c r="P20" s="3">
         <v>0.03</v>
       </c>
-      <c r="R20" s="13">
+      <c r="R20" s="12">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="U20" t="s">
+        <v>53</v>
+      </c>
+      <c r="V20">
+        <f>V11*V17</f>
+        <v>18.2</v>
+      </c>
+      <c r="W20">
+        <f>W11*W17</f>
+        <v>10</v>
+      </c>
+      <c r="X20">
+        <f>X11*X17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3">
         <v>100</v>
@@ -2059,10 +2281,10 @@
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="I21" s="3">
         <v>200</v>
@@ -2074,7 +2296,7 @@
         <v>10</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="O21" s="3">
         <v>1200</v>
@@ -2085,13 +2307,25 @@
       <c r="R21" s="12">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="V21">
+        <f>V12*V18</f>
+        <v>33</v>
+      </c>
+      <c r="W21">
+        <f>W12*W18</f>
+        <v>15</v>
+      </c>
+      <c r="X21">
+        <f>X12*X18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" spans="1:24">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3">
         <v>100</v>
@@ -2103,10 +2337,10 @@
         <v>50</v>
       </c>
       <c r="G22" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I22" s="10">
         <v>155</v>
@@ -2118,7 +2352,7 @@
         <v>20</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="O22" s="3">
         <v>3000</v>
@@ -2129,13 +2363,25 @@
       <c r="R22" s="12">
         <v>18</v>
       </c>
+      <c r="V22">
+        <f>V13*V19</f>
+        <v>51</v>
+      </c>
+      <c r="W22">
+        <f>W13*W19</f>
+        <v>20</v>
+      </c>
+      <c r="X22">
+        <f>X13*X19</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C23" s="3">
         <v>55</v>
@@ -2147,10 +2393,10 @@
         <v>5</v>
       </c>
       <c r="G23" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I23" s="7">
         <v>3000</v>
@@ -2167,10 +2413,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C24" s="3">
         <v>75</v>
@@ -2184,10 +2430,10 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C25" s="3">
         <v>200</v>
@@ -2201,10 +2447,10 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C26" s="7">
         <v>850</v>

</xml_diff>